<commit_message>
include license in test data
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/json_header.xlsx
+++ b/testdata/excel2json/excel2json_files/json_header.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools-uv/testdata/excel2json/new_excel2json_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374469-FE6E-6648-BE08-4EE49C65E73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E088F55F-4529-DB4E-AF36-237B38E07512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="6200" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
     <sheet name="Project" sheetId="2" r:id="rId2"/>
     <sheet name="Description" sheetId="3" r:id="rId3"/>
     <sheet name="Keywords" sheetId="4" r:id="rId4"/>
-    <sheet name="Users" sheetId="5" r:id="rId5"/>
+    <sheet name="Licenses" sheetId="6" r:id="rId5"/>
+    <sheet name="Users" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>prefixes</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>Liddell</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/public-domain</t>
   </si>
 </sst>
 </file>
@@ -6695,7 +6704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -14848,6 +14857,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C50B8C-3569-F046-A9DA-389E78D99920}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat(excel2json): allow null values for user passwords (DEV-5495) (#1996)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/json_header.xlsx
+++ b/testdata/excel2json/excel2json_files/json_header.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2json/excel2json_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E15175-1391-0D4F-B348-810824ABCAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16800375-CA07-7947-A2D2-756B61DB4339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="23340" windowHeight="10860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23580" yWindow="10920" windowWidth="23340" windowHeight="10860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>username</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Liddell</t>
-  </si>
-  <si>
-    <t>alice4322</t>
   </si>
   <si>
     <t>en</t>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t>Rabbit</t>
-  </si>
-  <si>
-    <t>alice8711</t>
   </si>
   <si>
     <t>fr</t>
@@ -676,10 +670,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -708,42 +702,42 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1752,7 +1746,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1767,16 +1761,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1803,16 +1797,16 @@
     </row>
     <row r="2" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6831,19 +6825,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -6869,13 +6863,13 @@
     </row>
     <row r="2" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -13888,7 +13882,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -13923,52 +13917,52 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14980,17 +14974,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -15005,7 +14999,9 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15072,60 +15068,56 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>